<commit_message>
Update to add TVS and ground plane
</commit_message>
<xml_diff>
--- a/PLACEMENT/Placement.xlsx
+++ b/PLACEMENT/Placement.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micro\Downloads\ESP32C6-2\PLACEMENT\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Micro\OneDrive\Projects\ZEUS Battery\ZeusController\PLACEMENT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3A8C5A-CAA0-4517-9964-1430F1401421}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C054CA3D-CB8A-4139-8B4D-BECE11B93007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57615" yWindow="240" windowWidth="19050" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19215" yWindow="240" windowWidth="38370" windowHeight="20505" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="23">
   <si>
     <t>Designator</t>
   </si>
@@ -61,10 +61,34 @@
     <t>U2</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
     <t>top</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>CR1</t>
+  </si>
+  <si>
+    <t>L1</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>R8</t>
+  </si>
+  <si>
+    <t>U3</t>
   </si>
 </sst>
 </file>
@@ -413,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D2" sqref="D2:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -450,13 +474,13 @@
         <v>5</v>
       </c>
       <c r="B2" s="2">
-        <v>150</v>
+        <v>149.302617</v>
       </c>
       <c r="C2" s="2">
-        <v>-67</v>
+        <v>-73.697383000000002</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E2" s="2">
         <v>-90</v>
@@ -467,16 +491,16 @@
         <v>6</v>
       </c>
       <c r="B3" s="2">
-        <v>150</v>
+        <v>141.658883</v>
       </c>
       <c r="C3" s="2">
-        <v>-73.4375</v>
+        <v>-70</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E3" s="2">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -484,16 +508,16 @@
         <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>115</v>
+        <v>116.94598499999999</v>
       </c>
       <c r="C4" s="2">
-        <v>-56</v>
+        <v>-56.339790999999998</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E4" s="2">
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -501,16 +525,16 @@
         <v>8</v>
       </c>
       <c r="B5" s="2">
-        <v>115</v>
+        <v>141.658883</v>
       </c>
       <c r="C5" s="2">
-        <v>-48</v>
+        <v>-72</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="2">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -518,84 +542,220 @@
         <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>150</v>
+        <v>149.52500000000001</v>
       </c>
       <c r="C6" s="2">
-        <v>-60.4375</v>
+        <v>-61</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E6" s="2">
-        <v>-90</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B7" s="2">
-        <v>139</v>
+        <v>117.94598499999999</v>
       </c>
       <c r="C7" s="2">
-        <v>-57</v>
+        <v>-56.339790999999998</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E7" s="2">
-        <v>180</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B8" s="2">
-        <v>125</v>
+        <v>142.14935</v>
       </c>
       <c r="C8" s="2">
-        <v>-47.655000000000001</v>
+        <v>-56.049999</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E8" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B9" s="2">
-        <v>143</v>
+        <v>145.85</v>
       </c>
       <c r="C9" s="2">
-        <v>-62</v>
+        <v>-70</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E9" s="2">
-        <v>90</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B10" s="2">
-        <v>143.52500000000001</v>
+        <v>125.985387</v>
       </c>
       <c r="C10" s="2">
-        <v>-71</v>
+        <v>-57.457653999999998</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E10" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="2">
+        <v>123.985387</v>
+      </c>
+      <c r="C11" s="2">
+        <v>-57.457653999999998</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="2">
+        <v>139</v>
+      </c>
+      <c r="C12" s="2">
+        <v>-56</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="2">
+        <v>117.68</v>
+      </c>
+      <c r="C13" s="2">
+        <v>-48</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="2">
+        <v>115.68</v>
+      </c>
+      <c r="C14" s="2">
+        <v>-48</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="2">
+        <v>144.534671</v>
+      </c>
+      <c r="C15" s="2">
+        <v>-74.026340000000005</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E15" s="2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="2">
+        <v>143.37078099999999</v>
+      </c>
+      <c r="C16" s="2">
+        <v>-74.059832999999998</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E16" s="2">
+        <v>-90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="2">
+        <v>144.52500000000001</v>
+      </c>
+      <c r="C17" s="2">
+        <v>-62</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" s="2">
         <v>180</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" s="2">
+        <v>147</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-75</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" s="2">
+        <v>-90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>